<commit_message>
make created json conform to eva_schema.json
</commit_message>
<xml_diff>
--- a/tests/resources/EVA_Submission_template.V1.1.4.xlsx
+++ b/tests/resources/EVA_Submission_template.V1.1.4.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="586">
   <si>
     <t xml:space="preserve">PLEASE READ FIRST</t>
   </si>
@@ -999,6 +999,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bastet normal sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Description</t>
   </si>
   <si>
     <t xml:space="preserve">Lemur catta</t>
@@ -2938,13 +2941,13 @@
         <v>78</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2952,10 +2955,10 @@
         <v>155</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2963,10 +2966,10 @@
         <v>160</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>287</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,10 +2977,10 @@
         <v>162</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6031,7 +6034,7 @@
   <sheetData>
     <row r="1" s="45" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="71" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D1" s="71" t="s">
         <v>15</v>
@@ -6057,15 +6060,15 @@
         <v>104</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>157</v>
@@ -6075,35 +6078,35 @@
       </c>
       <c r="F3" s="72"/>
       <c r="G3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>106</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>107</v>
@@ -6111,13 +6114,13 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>108</v>
@@ -6125,13 +6128,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>109</v>
@@ -6139,13 +6142,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>110</v>
@@ -6153,13 +6156,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>111</v>
@@ -6167,10 +6170,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>112</v>
@@ -6178,10 +6181,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>112</v>
@@ -6189,10 +6192,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>113</v>
@@ -6200,7 +6203,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>114</v>
@@ -6208,7 +6211,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>115</v>
@@ -6216,7 +6219,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>116</v>
@@ -6224,7 +6227,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>117</v>
@@ -6232,7 +6235,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>118</v>
@@ -6240,7 +6243,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>119</v>
@@ -6248,7 +6251,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>120</v>
@@ -6256,7 +6259,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>121</v>
@@ -6264,7 +6267,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>122</v>
@@ -6272,7 +6275,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>123</v>
@@ -6280,7 +6283,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>124</v>
@@ -6288,7 +6291,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>125</v>
@@ -6296,7 +6299,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>126</v>
@@ -6304,7 +6307,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>127</v>
@@ -6312,7 +6315,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>128</v>
@@ -6320,7 +6323,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>129</v>
@@ -6328,7 +6331,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>130</v>
@@ -6336,7 +6339,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>131</v>
@@ -6344,7 +6347,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>132</v>
@@ -6352,7 +6355,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>133</v>
@@ -6360,7 +6363,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>134</v>
@@ -6368,7 +6371,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>135</v>
@@ -6376,7 +6379,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>136</v>
@@ -6384,7 +6387,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>137</v>
@@ -6392,7 +6395,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>138</v>
@@ -6400,7 +6403,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>139</v>
@@ -6408,7 +6411,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>140</v>
@@ -6416,7 +6419,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>141</v>
@@ -6424,7 +6427,7 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>142</v>
@@ -6432,7 +6435,7 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>143</v>
@@ -6440,7 +6443,7 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>144</v>
@@ -6448,7 +6451,7 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>145</v>
@@ -6456,7 +6459,7 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>146</v>
@@ -6464,7 +6467,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>147</v>
@@ -6472,7 +6475,7 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>148</v>
@@ -6480,7 +6483,7 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>149</v>
@@ -6488,7 +6491,7 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>150</v>
@@ -6496,7 +6499,7 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>151</v>
@@ -6504,7 +6507,7 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>152</v>
@@ -6512,7 +6515,7 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>153</v>
@@ -6520,1148 +6523,1148 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E54" s="45"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B155" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B156" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B157" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B158" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B159" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B161" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B163" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B164" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B165" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B166" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B168" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B169" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B170" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B171" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B172" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B173" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B177" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B178" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B179" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B180" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B181" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B182" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B183" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B184" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B185" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B186" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B187" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B189" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B190" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B191" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B192" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B193" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B194" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B195" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B196" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B197" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B198" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B199" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B200" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B201" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B202" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B203" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B204" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B205" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B206" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B207" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B208" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B209" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B210" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B211" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B212" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B213" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B214" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B215" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B216" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B217" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B218" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B219" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B220" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B221" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B222" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B223" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B224" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B225" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B228" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B229" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B230" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B231" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B234" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B235" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B236" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B237" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B238" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B239" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B240" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B242" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B243" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B245" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B246" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B247" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B248" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B249" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B250" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B252" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B255" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B256" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B257" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B258" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B259" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B260" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B261" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B262" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B263" s="2" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B264" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B265" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B266" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B267" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B268" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B269" s="2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B270" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B271" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B272" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B273" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B274" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B275" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B276" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B277" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B278" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B279" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B280" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B281" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -13116,7 +13119,7 @@
   <dimension ref="A1:AR1007"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13425,7 +13428,9 @@
       <c r="E7" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="F7" s="29"/>
+      <c r="F7" s="29" t="s">
+        <v>275</v>
+      </c>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
@@ -13433,12 +13438,12 @@
         <v>9447</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
       <c r="N7" s="29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O7" s="29"/>
       <c r="P7" s="29"/>
@@ -13446,7 +13451,7 @@
       <c r="R7" s="29"/>
       <c r="S7" s="29"/>
       <c r="T7" s="29" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17553,31 +17558,31 @@
         <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>